<commit_message>
add data for lab 2
</commit_message>
<xml_diff>
--- a/fall2018/psyc5316/lab2/demographic.xlsx
+++ b/fall2018/psyc5316/lab2/demographic.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="440" windowWidth="28720" windowHeight="17560" tabRatio="500"/>
+    <workbookView xWindow="80" yWindow="440" windowWidth="10000" windowHeight="17560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
   <si>
     <t>subject</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t>f</t>
+  </si>
+  <si>
+    <t>m</t>
   </si>
 </sst>
 </file>
@@ -376,7 +379,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -433,15 +438,33 @@
       <c r="A5">
         <v>4</v>
       </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>21</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>19</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
add lab 2 data
</commit_message>
<xml_diff>
--- a/fall2018/psyc5316/lab2/demographic.xlsx
+++ b/fall2018/psyc5316/lab2/demographic.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="440" windowWidth="10000" windowHeight="17560" tabRatio="500"/>
+    <workbookView xWindow="17420" yWindow="440" windowWidth="10000" windowHeight="17560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="5">
   <si>
     <t>subject</t>
   </si>
@@ -380,7 +380,7 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -471,30 +471,66 @@
       <c r="A8">
         <v>7</v>
       </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>32</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>25</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>32</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11">
+        <v>28</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>34</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
update lab 2 data
</commit_message>
<xml_diff>
--- a/fall2018/psyc5316/lab2/demographic.xlsx
+++ b/fall2018/psyc5316/lab2/demographic.xlsx
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="5">
   <si>
     <t>subject</t>
   </si>
@@ -380,7 +380,7 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -537,15 +537,33 @@
       <c r="A14">
         <v>13</v>
       </c>
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>27</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15">
+        <v>29</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>